<commit_message>
add to openpyxl notebook
</commit_message>
<xml_diff>
--- a/sampleChart.xlsx
+++ b/sampleChart.xlsx
@@ -136,7 +136,7 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:t>My Chart</a:t>
+              <a:t>Cytokine array results</a:t>
             </a:r>
           </a:p>
         </rich>
@@ -150,7 +150,7 @@
           <idx val="0"/>
           <order val="0"/>
           <tx>
-            <v>First series</v>
+            <v>means</v>
           </tx>
           <spPr>
             <a:ln>
@@ -159,7 +159,7 @@
           </spPr>
           <val>
             <numRef>
-              <f>'Sheet'!$A$1:$A$10</f>
+              <f>'Sheet'!$B$2:$B$8</f>
             </numRef>
           </val>
         </ser>
@@ -203,9 +203,9 @@
 <wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
-      <col>2</col>
+      <col>4</col>
       <colOff>0</colOff>
-      <row>4</row>
+      <row>0</row>
       <rowOff>0</rowOff>
     </from>
     <ext cx="5400000" cy="2700000"/>
@@ -515,7 +515,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A10"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -524,53 +524,98 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="n">
-        <v>1</v>
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>names</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>means</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>stds</t>
+        </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>2</v>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>kkp</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0.1043081461209843</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.2601834427239736</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>3</v>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>srl</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0.03331519044931429</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.4971198541676912</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
-        <v>4</v>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>iok</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0.05019411593986726</v>
+      </c>
+      <c r="C4" t="n">
+        <v>2.669450422584103</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
-        <v>5</v>
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>nfm</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0.01011441930305049</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.7709364009354619</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
-        <v>6</v>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>uwz</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0.1067485493249866</v>
+      </c>
+      <c r="C6" t="n">
+        <v>1.255990664514469</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="n">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>10</v>
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>rjw</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0.05395380258988404</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.713453214246213</v>
       </c>
     </row>
   </sheetData>

</xml_diff>